<commit_message>
admin page for approval
</commit_message>
<xml_diff>
--- a/PUC Tracker.xlsx
+++ b/PUC Tracker.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1099969\OneDrive - Jabil\Desktop\Development_Project\Web\GitHub\PUC-V1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E94DAE-482A-4122-BAFD-03FE31045006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A89C37D-79EA-42F4-B176-E16CDAB756B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{D9DF3BC5-A219-488A-B707-D6423AA429FA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{D9DF3BC5-A219-488A-B707-D6423AA429FA}"/>
   </bookViews>
   <sheets>
     <sheet name="DatabaseTable" sheetId="1" r:id="rId1"/>
     <sheet name="Enhancement" sheetId="2" r:id="rId2"/>
     <sheet name="Menu" sheetId="3" r:id="rId3"/>
+    <sheet name="CounterUpdate" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="131">
   <si>
     <t>detailId</t>
   </si>
@@ -420,6 +421,15 @@
   </si>
   <si>
     <t>Part Mofidication</t>
+  </si>
+  <si>
+    <t>MachineName</t>
+  </si>
+  <si>
+    <t>RouteStep</t>
+  </si>
+  <si>
+    <t>custName</t>
   </si>
 </sst>
 </file>
@@ -812,7 +822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36536659-14FD-4079-9B4F-68A37DC0D68B}">
   <dimension ref="B1:R182"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -3675,4 +3685,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80F8C26-965F-4DB6-AB4E-405A5B89ECC7}">
+  <dimension ref="B3:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finish Request and Admin
</commit_message>
<xml_diff>
--- a/PUC Tracker.xlsx
+++ b/PUC Tracker.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1099969\OneDrive - Jabil\Desktop\Development_Project\Web\GitHub\PUC-V1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A89C37D-79EA-42F4-B176-E16CDAB756B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5653E7A2-B740-421E-811E-15087A1F18DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{D9DF3BC5-A219-488A-B707-D6423AA429FA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{D9DF3BC5-A219-488A-B707-D6423AA429FA}"/>
   </bookViews>
   <sheets>
     <sheet name="DatabaseTable" sheetId="1" r:id="rId1"/>
     <sheet name="Enhancement" sheetId="2" r:id="rId2"/>
-    <sheet name="Menu" sheetId="3" r:id="rId3"/>
-    <sheet name="CounterUpdate" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="Menu" sheetId="3" r:id="rId4"/>
+    <sheet name="CounterUpdate" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="160">
   <si>
     <t>detailId</t>
   </si>
@@ -430,13 +431,100 @@
   </si>
   <si>
     <t>custName</t>
+  </si>
+  <si>
+    <t>00906212011427|Quality Inspection SCH_PCBA_B2BAY18_COATING TOP|SND PCBA Route 07|QC SCH_COATING_T|3/28/2022 8:53:59 AM|3/28/2022 8:53:59 AM|13|HCM_SCHNEIDER</t>
+  </si>
+  <si>
+    <t>BFT</t>
+  </si>
+  <si>
+    <t>RFT</t>
+  </si>
+  <si>
+    <t>CONFIG</t>
+  </si>
+  <si>
+    <t>DTT</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>APTC</t>
+  </si>
+  <si>
+    <t>Email triggering on detail part added</t>
+  </si>
+  <si>
+    <t>Email triggering on machine/fixture added</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Will use PBI instead</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>CRD</t>
+  </si>
+  <si>
+    <t>Analysis Date</t>
+  </si>
+  <si>
+    <t>Power BI</t>
+  </si>
+  <si>
+    <t>webpage / Edwin Script</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>count as 1</t>
+  </si>
+  <si>
+    <t>not ok</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>different</t>
+  </si>
+  <si>
+    <t>count as 2</t>
+  </si>
+  <si>
+    <t>SN1</t>
+  </si>
+  <si>
+    <t>PN1</t>
+  </si>
+  <si>
+    <t>CRD1</t>
+  </si>
+  <si>
+    <t>Analysis Date1</t>
+  </si>
+  <si>
+    <t>Analysis Date2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,8 +532,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,8 +565,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -494,11 +595,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -506,6 +642,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3466,19 +3621,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF29C7F6-4DB4-44E8-8455-8E338FEC0723}">
-  <dimension ref="A3:C11"/>
+  <dimension ref="A3:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B11" sqref="B11:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="37.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -3488,16 +3644,22 @@
       <c r="C3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>97</v>
       </c>
@@ -3505,40 +3667,65 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>99</v>
       </c>
       <c r="C6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>100</v>
       </c>
       <c r="C7" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3547,11 +3734,175 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A55C4D7-CDB9-4B84-B6ED-ED5E31AC91B8}">
+  <dimension ref="E6:M15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E7" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10">
+        <v>2</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E9" s="12">
+        <v>2</v>
+      </c>
+      <c r="F9" s="10">
+        <v>2</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E10" s="12">
+        <v>3</v>
+      </c>
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="14" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E14" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E15" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF894900-568A-4BAA-B8A2-76851BB63D25}">
   <dimension ref="B2:C18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3687,20 +4038,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80F8C26-965F-4DB6-AB4E-405A5B89ECC7}">
-  <dimension ref="B3:E6"/>
+  <dimension ref="B1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+    </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>24</v>
@@ -3716,22 +4073,80 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>13</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>13</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>14</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="2">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="2">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="2">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="2">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="2">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>